<commit_message>
Remise en ordre des TD et TP du groupe 2.
</commit_message>
<xml_diff>
--- a/AnAn.xlsx
+++ b/AnAn.xlsx
@@ -307,14 +307,14 @@
         <v>4</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E13" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s" s="0">
         <v>16</v>
@@ -332,14 +332,14 @@
         <v>4</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E14" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F14" s="0"/>
       <c r="G14" t="s" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H14" t="s" s="0">
         <v>16</v>
@@ -924,14 +924,14 @@
         <v>4</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E59" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F59" s="0"/>
       <c r="G59" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H59" t="s" s="0">
         <v>16</v>
@@ -949,14 +949,14 @@
         <v>4</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E60" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F60" s="0"/>
       <c r="G60" t="s" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H60" t="s" s="0">
         <v>16</v>

</xml_diff>